<commit_message>
docs: add excel file
</commit_message>
<xml_diff>
--- a/Guru99Bank/data/Datos_LoginGuru99.xlsx
+++ b/Guru99Bank/data/Datos_LoginGuru99.xlsx
@@ -35,17 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>1q2w3e4r</t>
   </si>
   <si>
-    <t>4et45ete</t>
-  </si>
-  <si>
-    <t>regsergfea&amp;/</t>
-  </si>
-  <si>
     <t>mngr533450</t>
   </si>
   <si>
@@ -55,10 +49,10 @@
     <t>mngr533455</t>
   </si>
   <si>
-    <t>mngr533444</t>
-  </si>
-  <si>
-    <t>mngr533459</t>
+    <t>v</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
@@ -79,24 +73,12 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,12 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -433,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,36 +423,37 @@
     <col min="1" max="2" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>